<commit_message>
add filenames and missing composer
</commit_message>
<xml_diff>
--- a/workList.xlsx
+++ b/workList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laney\Documents\GitHub\viz-classical-music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC2BD58-47C5-48B2-A8AF-0E71C01594C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B84F30-5B65-4A92-850D-78B4B3DADA98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1600" windowWidth="14400" windowHeight="8260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="153">
   <si>
     <t>file</t>
   </si>
@@ -294,9 +294,6 @@
     <t>victoria</t>
   </si>
   <si>
-    <t>variations-2.krn</t>
-  </si>
-  <si>
     <t>morales</t>
   </si>
   <si>
@@ -481,6 +478,12 @@
   </si>
   <si>
     <t>classify as strings or keys?</t>
+  </si>
+  <si>
+    <t>variations-2_edited.krn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added missing instrumentation (piano) to .krn spines. Instrumentation was in the AIN record but not recognized by music21.  </t>
   </si>
 </sst>
 </file>
@@ -810,7 +813,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,10 +838,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -860,16 +863,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -877,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -891,16 +894,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -908,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -936,16 +939,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -953,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -981,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -995,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -1065,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1079,10 +1082,10 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1090,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -1112,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -1123,13 +1126,13 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1148,13 +1151,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1162,13 +1165,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" t="s">
         <v>144</v>
-      </c>
-      <c r="E25" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1187,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
         <v>48</v>
@@ -1209,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -1245,10 +1248,10 @@
         <v>56</v>
       </c>
       <c r="C32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" t="s">
         <v>131</v>
-      </c>
-      <c r="E32" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1259,10 +1262,10 @@
         <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1270,7 +1273,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
         <v>58</v>
@@ -1281,16 +1284,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" t="s">
         <v>134</v>
       </c>
-      <c r="E35" t="s">
-        <v>135</v>
-      </c>
       <c r="F35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1298,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
         <v>59</v>
@@ -1312,10 +1315,10 @@
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1334,13 +1337,13 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
         <v>90</v>
       </c>
-      <c r="C39" t="s">
-        <v>91</v>
-      </c>
       <c r="E39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1359,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
         <v>65</v>
@@ -1370,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1384,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
         <v>66</v>
@@ -1428,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1439,13 +1442,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1467,10 +1470,10 @@
         <v>75</v>
       </c>
       <c r="C50" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" t="s">
         <v>148</v>
-      </c>
-      <c r="E50" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -1478,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51" t="s">
         <v>76</v>
@@ -1489,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C52" t="s">
         <v>77</v>
@@ -1500,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
         <v>78</v>
@@ -1511,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
         <v>79</v>
@@ -1544,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C57" t="s">
         <v>84</v>
@@ -1561,10 +1564,10 @@
         <v>85</v>
       </c>
       <c r="E58" t="s">
+        <v>149</v>
+      </c>
+      <c r="F58" t="s">
         <v>150</v>
-      </c>
-      <c r="F58" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -1572,7 +1575,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
         <v>87</v>
@@ -1586,10 +1589,10 @@
         <v>88</v>
       </c>
       <c r="C60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -1597,10 +1600,13 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>89</v>
+        <v>151</v>
+      </c>
+      <c r="E61" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add features, update file naming conventions
</commit_message>
<xml_diff>
--- a/workList.xlsx
+++ b/workList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laney\Documents\GitHub\viz-classical-music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B84F30-5B65-4A92-850D-78B4B3DADA98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3FEB20-A47D-4572-8807-D8C4DC8B6A6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32385" yWindow="1755" windowWidth="17730" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="155">
   <si>
     <t>file</t>
   </si>
@@ -168,9 +168,6 @@
     <t>hofmann</t>
   </si>
   <si>
-    <t>schelm.krn</t>
-  </si>
-  <si>
     <t>prelude67-14.krn</t>
   </si>
   <si>
@@ -471,9 +468,6 @@
     <t>sonno_edited.krn</t>
   </si>
   <si>
-    <t>Added *Ivox to kern spines because instrumentation format was not recognized by music21 (e.g. *I"Bassus)</t>
-  </si>
-  <si>
     <t>This piece has a hurdy-gurdy, which is not recognized in music21</t>
   </si>
   <si>
@@ -484,6 +478,18 @@
   </si>
   <si>
     <t xml:space="preserve">Added missing instrumentation (piano) to .krn spines. Instrumentation was in the AIN record but not recognized by music21.  </t>
+  </si>
+  <si>
+    <t>schelm_edited.krn</t>
+  </si>
+  <si>
+    <t>No tempo marking. IMSLP version marked allegro. Added tempo marking of 130.</t>
+  </si>
+  <si>
+    <t>Added *Ivox to kern spines because instrumentation format was not recognized by music21 (e.g. *I"Bassus). Also added missing tempo marking of 60 based on IMSLP version.</t>
+  </si>
+  <si>
+    <t>Added missing instrumentation (vocals) to .krn spines.  No tempo marking, could not find one in IMSLP or choralwiki versions. Added tempo of 60.</t>
   </si>
 </sst>
 </file>
@@ -812,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
@@ -838,10 +844,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -863,16 +869,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -880,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -894,16 +900,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -911,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -939,16 +945,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -956,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -984,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -998,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -1068,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1082,10 +1088,10 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1093,7 +1099,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -1115,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -1126,13 +1132,13 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1151,13 +1157,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1165,13 +1171,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" t="s">
         <v>143</v>
-      </c>
-      <c r="E25" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1182,7 +1188,10 @@
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>151</v>
+      </c>
+      <c r="E26" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1190,10 +1199,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1201,10 +1210,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1212,10 +1221,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1223,10 +1232,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
         <v>52</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1234,10 +1243,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
         <v>54</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1245,13 +1254,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" t="s">
         <v>130</v>
-      </c>
-      <c r="E32" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1259,13 +1268,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1273,10 +1282,10 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1284,16 +1293,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" t="s">
         <v>133</v>
       </c>
-      <c r="E35" t="s">
-        <v>134</v>
-      </c>
       <c r="F35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1301,10 +1310,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1312,13 +1321,13 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1326,10 +1335,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1337,13 +1346,13 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" t="s">
         <v>89</v>
       </c>
-      <c r="C39" t="s">
-        <v>90</v>
-      </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1351,10 +1360,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
         <v>63</v>
-      </c>
-      <c r="C40" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1362,10 +1371,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1373,13 +1382,13 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1387,10 +1396,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1398,10 +1407,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1409,10 +1418,10 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1420,10 +1429,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -1431,10 +1440,10 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1442,13 +1451,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1456,10 +1465,10 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" t="s">
         <v>73</v>
-      </c>
-      <c r="C49" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -1467,13 +1476,13 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E50" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -1481,10 +1490,10 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -1492,10 +1501,10 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -1503,10 +1512,10 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -1514,10 +1523,10 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -1525,10 +1534,10 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" t="s">
         <v>80</v>
-      </c>
-      <c r="C55" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -1536,10 +1545,10 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" t="s">
         <v>82</v>
-      </c>
-      <c r="C56" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -1547,10 +1556,10 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -1558,16 +1567,16 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E58" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -1575,10 +1584,10 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -1586,13 +1595,13 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E60" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -1600,13 +1609,13 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C61" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E61" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>